<commit_message>
New models trained for vis-nir1-nir2
</commit_message>
<xml_diff>
--- a/v3.0/datasets/ASPECT/REF_MEAS_upd_wl.xlsx
+++ b/v3.0/datasets/ASPECT/REF_MEAS_upd_wl.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radsaga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valtterimj/Downloads/Työ/Aalto/Hera/Pipeline/Asteroid-spectra/v3.0/datasets/ASPECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F144B73-D8A6-45E1-982D-3EB875CF13E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FF8B8C-E107-AA40-AC88-94A65BBBA36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B7B7263-57CE-4670-B472-5AB98268D44C}"/>
+    <workbookView xWindow="12120" yWindow="660" windowWidth="16520" windowHeight="16040" activeTab="1" xr2:uid="{3B7B7263-57CE-4670-B472-5AB98268D44C}"/>
   </bookViews>
   <sheets>
     <sheet name="600W, 10000|2500, LO" sheetId="1" r:id="rId1"/>
-    <sheet name="600W, 10000|2500, HO" sheetId="2" r:id="rId2"/>
-    <sheet name="400W, 10000|2500, LO" sheetId="3" r:id="rId3"/>
-    <sheet name="400W, 10000|2500, HO" sheetId="4" r:id="rId4"/>
-    <sheet name="200W, 10000|2500, LO" sheetId="5" r:id="rId5"/>
-    <sheet name="200W, 10000|2500, HO" sheetId="6" r:id="rId6"/>
-    <sheet name="600W, 7500|1875, LO" sheetId="7" r:id="rId7"/>
-    <sheet name="600W, 7500|1875, HO" sheetId="8" r:id="rId8"/>
-    <sheet name="600W, 5000|1250, LO" sheetId="9" r:id="rId9"/>
-    <sheet name="600W, 5000|1250, HO" sheetId="10" r:id="rId10"/>
+    <sheet name="ASPECT default wl" sheetId="11" r:id="rId2"/>
+    <sheet name="600W, 10000|2500, HO" sheetId="2" r:id="rId3"/>
+    <sheet name="400W, 10000|2500, LO" sheetId="3" r:id="rId4"/>
+    <sheet name="400W, 10000|2500, HO" sheetId="4" r:id="rId5"/>
+    <sheet name="200W, 10000|2500, LO" sheetId="5" r:id="rId6"/>
+    <sheet name="200W, 10000|2500, HO" sheetId="6" r:id="rId7"/>
+    <sheet name="600W, 7500|1875, LO" sheetId="7" r:id="rId8"/>
+    <sheet name="600W, 7500|1875, HO" sheetId="8" r:id="rId9"/>
+    <sheet name="600W, 5000|1250, LO" sheetId="9" r:id="rId10"/>
+    <sheet name="600W, 5000|1250, HO" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="47">
   <si>
     <t>NIR1</t>
   </si>
@@ -126,6 +127,66 @@
   </si>
   <si>
     <t>wl</t>
+  </si>
+  <si>
+    <t>904.1666667</t>
+  </si>
+  <si>
+    <t>933.3333333</t>
+  </si>
+  <si>
+    <t>962.5</t>
+  </si>
+  <si>
+    <t>991.6666667</t>
+  </si>
+  <si>
+    <t>1020.833333</t>
+  </si>
+  <si>
+    <t>1079.166667</t>
+  </si>
+  <si>
+    <t>1108.333333</t>
+  </si>
+  <si>
+    <t>1137.5</t>
+  </si>
+  <si>
+    <t>1166.666667</t>
+  </si>
+  <si>
+    <t>1195.833333</t>
+  </si>
+  <si>
+    <t>1254.166667</t>
+  </si>
+  <si>
+    <t>1283.333333</t>
+  </si>
+  <si>
+    <t>1312.5</t>
+  </si>
+  <si>
+    <t>1341.666667</t>
+  </si>
+  <si>
+    <t>1370.833333</t>
+  </si>
+  <si>
+    <t>1429.166667</t>
+  </si>
+  <si>
+    <t>1458.333333</t>
+  </si>
+  <si>
+    <t>1487.5</t>
+  </si>
+  <si>
+    <t>1516.666667</t>
+  </si>
+  <si>
+    <t>1545.833333</t>
   </si>
 </sst>
 </file>
@@ -499,18 +560,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B3972A-39D5-4BAB-AAD9-004981E85E6A}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -521,7 +582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -547,7 +608,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.32861793</v>
       </c>
@@ -579,7 +640,7 @@
         <v>681.25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.32263425000000001</v>
       </c>
@@ -608,7 +669,7 @@
         <v>712.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.32816434999999999</v>
       </c>
@@ -637,7 +698,7 @@
         <v>743.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.31767706000000001</v>
       </c>
@@ -666,7 +727,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.29767901000000002</v>
       </c>
@@ -695,7 +756,7 @@
         <v>806.25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.29737683999999998</v>
       </c>
@@ -724,7 +785,7 @@
         <v>837.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.27354183999999998</v>
       </c>
@@ -753,7 +814,7 @@
         <v>868.75</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.26351903999999998</v>
       </c>
@@ -785,7 +846,7 @@
         <v>880.77</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.26064894999999999</v>
       </c>
@@ -814,7 +875,7 @@
         <v>911.54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.25988728</v>
       </c>
@@ -843,7 +904,7 @@
         <v>942.31</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.25910275999999999</v>
       </c>
@@ -872,7 +933,7 @@
         <v>973.08</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26015595000000002</v>
       </c>
@@ -901,7 +962,7 @@
         <v>1003.85</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26324261999999998</v>
       </c>
@@ -930,7 +991,7 @@
         <v>1034.6199999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26693902000000003</v>
       </c>
@@ -959,7 +1020,7 @@
         <v>1065.3900000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.27342362999999997</v>
       </c>
@@ -988,7 +1049,7 @@
         <v>1096.1600000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27831178000000001</v>
       </c>
@@ -1017,7 +1078,7 @@
         <v>1126.93</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.28418383000000003</v>
       </c>
@@ -1046,7 +1107,7 @@
         <v>1157.7</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.2886186</v>
       </c>
@@ -1075,7 +1136,7 @@
         <v>1188.47</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.28980823</v>
       </c>
@@ -1104,7 +1165,7 @@
         <v>1219.24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.29152222999999999</v>
       </c>
@@ -1136,7 +1197,7 @@
         <v>1230.77</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.29004333999999998</v>
       </c>
@@ -1165,7 +1226,7 @@
         <v>1261.54</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.29422211999999998</v>
       </c>
@@ -1194,7 +1255,7 @@
         <v>1292.31</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29798270999999998</v>
       </c>
@@ -1223,7 +1284,7 @@
         <v>1323.08</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29901745000000002</v>
       </c>
@@ -1252,7 +1313,7 @@
         <v>1353.85</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.30299796000000001</v>
       </c>
@@ -1281,7 +1342,7 @@
         <v>1384.62</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.31520384000000001</v>
       </c>
@@ -1310,7 +1371,7 @@
         <v>1415.39</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.31941060999999998</v>
       </c>
@@ -1339,7 +1400,7 @@
         <v>1446.16</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.32004807000000002</v>
       </c>
@@ -1368,7 +1429,7 @@
         <v>1476.93</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.32258165</v>
       </c>
@@ -1397,7 +1458,7 @@
         <v>1507.7</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.32038322000000002</v>
       </c>
@@ -1426,7 +1487,7 @@
         <v>1538.47</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.31695635</v>
       </c>
@@ -1461,6 +1522,872 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2FAC0B-EE3B-42E4-A7E5-2FA82B54F342}">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.33089004999999999</v>
+      </c>
+      <c r="B6">
+        <v>0.20646750999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.28629504</v>
+      </c>
+      <c r="D6">
+        <v>0.28629504</v>
+      </c>
+      <c r="G6">
+        <v>0.12811826000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.14733599999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.14758238000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.13575608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.32077763999999998</v>
+      </c>
+      <c r="B7">
+        <v>0.21652490999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.28092345000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.29161604000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.13584446999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.14167679</v>
+      </c>
+      <c r="I7">
+        <v>0.14872418000000001</v>
+      </c>
+      <c r="J7">
+        <v>0.13803159000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.31667183999999998</v>
+      </c>
+      <c r="B8">
+        <v>0.2116113</v>
+      </c>
+      <c r="C8">
+        <v>0.29655387</v>
+      </c>
+      <c r="D8">
+        <v>0.28810928000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.13660354</v>
+      </c>
+      <c r="H8">
+        <v>0.13635517</v>
+      </c>
+      <c r="I8">
+        <v>0.13983234999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.13585843</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.32184238999999998</v>
+      </c>
+      <c r="B9">
+        <v>0.21907161</v>
+      </c>
+      <c r="C9">
+        <v>0.28096438000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.28038863000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.13098236999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.14134580999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.14019430999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.12810363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.30941286000000001</v>
+      </c>
+      <c r="B10">
+        <v>0.20577819</v>
+      </c>
+      <c r="C10">
+        <v>0.27250699</v>
+      </c>
+      <c r="D10">
+        <v>0.27287978000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.13159366</v>
+      </c>
+      <c r="H10">
+        <v>0.14464119</v>
+      </c>
+      <c r="I10">
+        <v>0.13643989000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.14575954999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.28771482999999998</v>
+      </c>
+      <c r="B11">
+        <v>0.19554424000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.23169955</v>
+      </c>
+      <c r="D11">
+        <v>0.24595798999999999</v>
+      </c>
+      <c r="G11">
+        <v>9.9299810000000002E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.13952896000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.11763208</v>
+      </c>
+      <c r="J11">
+        <v>0.12068746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.29838998</v>
+      </c>
+      <c r="B12">
+        <v>0.18175313000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.26833631000000002</v>
+      </c>
+      <c r="D12">
+        <v>0.24758496999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.11234347</v>
+      </c>
+      <c r="H12">
+        <v>0.12593918000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.14311270000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.12307692000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.26548012999999998</v>
+      </c>
+      <c r="B15">
+        <v>0.22094370999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.23038079</v>
+      </c>
+      <c r="D15">
+        <v>0.23791391000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.12847681999999999</v>
+      </c>
+      <c r="H15">
+        <v>0.13899006999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.12152317999999999</v>
+      </c>
+      <c r="J15">
+        <v>0.13269868000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.27439933999999999</v>
+      </c>
+      <c r="B16">
+        <v>0.22336370999999999</v>
+      </c>
+      <c r="C16">
+        <v>0.23491537000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.24627767</v>
+      </c>
+      <c r="G16">
+        <v>0.12934075</v>
+      </c>
+      <c r="H16">
+        <v>0.13871464</v>
+      </c>
+      <c r="I16">
+        <v>0.11987217</v>
+      </c>
+      <c r="J16">
+        <v>0.13454847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.26748034999999998</v>
+      </c>
+      <c r="B17">
+        <v>0.22184003999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.22901526</v>
+      </c>
+      <c r="D17">
+        <v>0.24114656000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.12737863999999999</v>
+      </c>
+      <c r="H17">
+        <v>0.13618122999999999</v>
+      </c>
+      <c r="I17">
+        <v>0.11968562000000001</v>
+      </c>
+      <c r="J17">
+        <v>0.13129911999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.26209485999999999</v>
+      </c>
+      <c r="B18">
+        <v>0.21396032000000001</v>
+      </c>
+      <c r="C18">
+        <v>0.22650012</v>
+      </c>
+      <c r="D18">
+        <v>0.23459874</v>
+      </c>
+      <c r="G18">
+        <v>0.12722670999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.13480284000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.12245898</v>
+      </c>
+      <c r="J18">
+        <v>0.13251694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.26120821999999999</v>
+      </c>
+      <c r="B19">
+        <v>0.21416742999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.22913217</v>
+      </c>
+      <c r="D19">
+        <v>0.23643053999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.13014413</v>
+      </c>
+      <c r="H19">
+        <v>0.13750382999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.12486967</v>
+      </c>
+      <c r="J19">
+        <v>0.13351732999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.26752530000000002</v>
+      </c>
+      <c r="B20">
+        <v>0.22079117000000001</v>
+      </c>
+      <c r="C20">
+        <v>0.23563323999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.24225698000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.13529591999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.14308493999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.12977614000000001</v>
+      </c>
+      <c r="J20">
+        <v>0.13854646000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.27011866000000001</v>
+      </c>
+      <c r="B21">
+        <v>0.22357836</v>
+      </c>
+      <c r="C21">
+        <v>0.24083834000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.24650948</v>
+      </c>
+      <c r="G21">
+        <v>0.13826475999999999</v>
+      </c>
+      <c r="H21">
+        <v>0.14652488999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.13321005</v>
+      </c>
+      <c r="J21">
+        <v>0.14140854</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.27199624999999999</v>
+      </c>
+      <c r="B22">
+        <v>0.22459208</v>
+      </c>
+      <c r="C22">
+        <v>0.2427668</v>
+      </c>
+      <c r="D22">
+        <v>0.25319697000000002</v>
+      </c>
+      <c r="G22">
+        <v>0.13859004999999999</v>
+      </c>
+      <c r="H22">
+        <v>0.14758373</v>
+      </c>
+      <c r="I22">
+        <v>0.13434304</v>
+      </c>
+      <c r="J22">
+        <v>0.14383636999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.28171053000000001</v>
+      </c>
+      <c r="B23">
+        <v>0.23190789000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.24881579000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.26078947000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.14467105</v>
+      </c>
+      <c r="H23">
+        <v>0.15269737</v>
+      </c>
+      <c r="I23">
+        <v>0.13717104999999999</v>
+      </c>
+      <c r="J23">
+        <v>0.14611842</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.28868268000000002</v>
+      </c>
+      <c r="B24">
+        <v>0.23567774</v>
+      </c>
+      <c r="C24">
+        <v>0.25600555000000003</v>
+      </c>
+      <c r="D24">
+        <v>0.26627351999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.14513919</v>
+      </c>
+      <c r="H24">
+        <v>0.15367270999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.13924204000000001</v>
+      </c>
+      <c r="J24">
+        <v>0.14964876999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.29242199000000002</v>
+      </c>
+      <c r="B25">
+        <v>0.24279345999999999</v>
+      </c>
+      <c r="C25">
+        <v>0.25995541999999999</v>
+      </c>
+      <c r="D25">
+        <v>0.27280831999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.14977712000000001</v>
+      </c>
+      <c r="H25">
+        <v>0.15713224000000001</v>
+      </c>
+      <c r="I25">
+        <v>0.14108470000000001</v>
+      </c>
+      <c r="J25">
+        <v>0.15022288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.29024002999999998</v>
+      </c>
+      <c r="B26">
+        <v>0.24278311999999999</v>
+      </c>
+      <c r="C26">
+        <v>0.26190123999999998</v>
+      </c>
+      <c r="D26">
+        <v>0.27433647</v>
+      </c>
+      <c r="G26">
+        <v>0.15099926</v>
+      </c>
+      <c r="H26">
+        <v>0.16064291</v>
+      </c>
+      <c r="I26">
+        <v>0.14194776000000001</v>
+      </c>
+      <c r="J26">
+        <v>0.15404461999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.30381944</v>
+      </c>
+      <c r="B29">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="C29">
+        <v>0.26163194000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.27916667000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.15121528000000001</v>
+      </c>
+      <c r="H29">
+        <v>0.16371527999999999</v>
+      </c>
+      <c r="I29">
+        <v>0.15885416999999999</v>
+      </c>
+      <c r="J29">
+        <v>0.15468750000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0.29318894000000001</v>
+      </c>
+      <c r="B30">
+        <v>0.25830721000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.26058705999999998</v>
+      </c>
+      <c r="D30">
+        <v>0.28201767</v>
+      </c>
+      <c r="G30">
+        <v>0.14636648999999999</v>
+      </c>
+      <c r="H30">
+        <v>0.15822172000000001</v>
+      </c>
+      <c r="I30">
+        <v>0.1461385</v>
+      </c>
+      <c r="J30">
+        <v>0.15252209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0.29888334999999999</v>
+      </c>
+      <c r="B31">
+        <v>0.25801853000000002</v>
+      </c>
+      <c r="C31">
+        <v>0.26666666999999999</v>
+      </c>
+      <c r="D31">
+        <v>0.28168210999999999</v>
+      </c>
+      <c r="G31">
+        <v>0.15633167000000001</v>
+      </c>
+      <c r="H31">
+        <v>0.16345925</v>
+      </c>
+      <c r="I31">
+        <v>0.15452601999999999</v>
+      </c>
+      <c r="J31">
+        <v>0.15481112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.30217259000000002</v>
+      </c>
+      <c r="B32">
+        <v>0.25760408000000001</v>
+      </c>
+      <c r="C32">
+        <v>0.27080956</v>
+      </c>
+      <c r="D32">
+        <v>0.28508314000000001</v>
+      </c>
+      <c r="G32">
+        <v>0.15933973000000001</v>
+      </c>
+      <c r="H32">
+        <v>0.16380628999999999</v>
+      </c>
+      <c r="I32">
+        <v>0.15516446</v>
+      </c>
+      <c r="J32">
+        <v>0.15730063999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.30705962999999997</v>
+      </c>
+      <c r="B33">
+        <v>0.26319397</v>
+      </c>
+      <c r="C33">
+        <v>0.27777930000000001</v>
+      </c>
+      <c r="D33">
+        <v>0.28655243000000002</v>
+      </c>
+      <c r="G33">
+        <v>0.15824537</v>
+      </c>
+      <c r="H33">
+        <v>0.16394791</v>
+      </c>
+      <c r="I33">
+        <v>0.15824537</v>
+      </c>
+      <c r="J33">
+        <v>0.15901302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0.30741971000000001</v>
+      </c>
+      <c r="B34">
+        <v>0.27033697000000001</v>
+      </c>
+      <c r="C34">
+        <v>0.28071508000000001</v>
+      </c>
+      <c r="D34">
+        <v>0.29463692000000002</v>
+      </c>
+      <c r="G34">
+        <v>0.1642778</v>
+      </c>
+      <c r="H34">
+        <v>0.16971997999999999</v>
+      </c>
+      <c r="I34">
+        <v>0.15870907000000001</v>
+      </c>
+      <c r="J34">
+        <v>0.16174656000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0.31991944999999999</v>
+      </c>
+      <c r="B35">
+        <v>0.28286624999999999</v>
+      </c>
+      <c r="C35">
+        <v>0.29065278999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.30219836</v>
+      </c>
+      <c r="G35">
+        <v>0.16271186000000001</v>
+      </c>
+      <c r="H35">
+        <v>0.17210940999999999</v>
+      </c>
+      <c r="I35">
+        <v>0.16123510999999999</v>
+      </c>
+      <c r="J35">
+        <v>0.16338311999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.31824637</v>
+      </c>
+      <c r="B36">
+        <v>0.27761655000000002</v>
+      </c>
+      <c r="C36">
+        <v>0.28342081000000002</v>
+      </c>
+      <c r="D36">
+        <v>0.30392096000000002</v>
+      </c>
+      <c r="G36">
+        <v>0.16251930000000001</v>
+      </c>
+      <c r="H36">
+        <v>0.16696511</v>
+      </c>
+      <c r="I36">
+        <v>0.15844395999999999</v>
+      </c>
+      <c r="J36">
+        <v>0.15906144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0.32429448</v>
+      </c>
+      <c r="B37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C37">
+        <v>0.29006135</v>
+      </c>
+      <c r="D37">
+        <v>0.30380368000000002</v>
+      </c>
+      <c r="G37">
+        <v>0.16036810000000001</v>
+      </c>
+      <c r="H37">
+        <v>0.17092025</v>
+      </c>
+      <c r="I37">
+        <v>0.15840491000000001</v>
+      </c>
+      <c r="J37">
+        <v>0.16343558</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.33208990999999999</v>
+      </c>
+      <c r="B38">
+        <v>0.28592380000000001</v>
+      </c>
+      <c r="C38">
+        <v>0.29689144000000001</v>
+      </c>
+      <c r="D38">
+        <v>0.30862425999999998</v>
+      </c>
+      <c r="G38">
+        <v>0.16617249000000001</v>
+      </c>
+      <c r="H38">
+        <v>0.1733142</v>
+      </c>
+      <c r="I38">
+        <v>0.16349433999999999</v>
+      </c>
+      <c r="J38">
+        <v>0.16362187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.33449812000000001</v>
+      </c>
+      <c r="B39">
+        <v>0.29133265000000003</v>
+      </c>
+      <c r="C39">
+        <v>0.30325454000000002</v>
+      </c>
+      <c r="D39">
+        <v>0.31147652999999997</v>
+      </c>
+      <c r="G39">
+        <v>0.16553614</v>
+      </c>
+      <c r="H39">
+        <v>0.1744433</v>
+      </c>
+      <c r="I39">
+        <v>0.16073998</v>
+      </c>
+      <c r="J39">
+        <v>0.16635833999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.32315044999999998</v>
+      </c>
+      <c r="B40">
+        <v>0.28308162999999997</v>
+      </c>
+      <c r="C40">
+        <v>0.29302236999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.31091569000000002</v>
+      </c>
+      <c r="G40">
+        <v>0.16486331000000001</v>
+      </c>
+      <c r="H40">
+        <v>0.17403937999999999</v>
+      </c>
+      <c r="I40">
+        <v>0.16409863999999999</v>
+      </c>
+      <c r="J40">
+        <v>0.15935768</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F580E-9841-4024-8794-350037C7121D}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -1468,9 +2395,9 @@
       <selection activeCell="G5" sqref="G5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1481,7 +2408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +2416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +2442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.33094245</v>
       </c>
@@ -1541,7 +2468,7 @@
         <v>0.14211842999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.32504317999999999</v>
       </c>
@@ -1567,7 +2494,7 @@
         <v>0.13886009999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.31379149000000001</v>
       </c>
@@ -1593,7 +2520,7 @@
         <v>0.13987844999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.34007738999999998</v>
       </c>
@@ -1619,7 +2546,7 @@
         <v>0.13399668000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.32463767999999998</v>
       </c>
@@ -1645,7 +2572,7 @@
         <v>0.13596838</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.3068323</v>
       </c>
@@ -1671,7 +2598,7 @@
         <v>0.13726708000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.29695946000000001</v>
       </c>
@@ -1697,7 +2624,7 @@
         <v>0.12804054000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26625788</v>
       </c>
@@ -1723,7 +2650,7 @@
         <v>0.13408278000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.27157605000000001</v>
       </c>
@@ -1749,7 +2676,7 @@
         <v>0.13241569</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26429009999999997</v>
       </c>
@@ -1775,7 +2702,7 @@
         <v>0.13079287000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26531403999999997</v>
       </c>
@@ -1801,7 +2728,7 @@
         <v>0.13534238000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26443707999999999</v>
       </c>
@@ -1827,7 +2754,7 @@
         <v>0.13216088000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26569978</v>
       </c>
@@ -1853,7 +2780,7 @@
         <v>0.13981146</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27062591000000003</v>
       </c>
@@ -1879,7 +2806,7 @@
         <v>0.1426492</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.27602979</v>
       </c>
@@ -1905,7 +2832,7 @@
         <v>0.14822921</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28470023999999999</v>
       </c>
@@ -1931,7 +2858,7 @@
         <v>0.15002398</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.29505247000000001</v>
       </c>
@@ -1957,7 +2884,7 @@
         <v>0.15259037</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.29294974000000001</v>
       </c>
@@ -1983,7 +2910,7 @@
         <v>0.15684603</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.29491313000000002</v>
       </c>
@@ -2009,7 +2936,7 @@
         <v>0.15256437</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29729729999999999</v>
       </c>
@@ -2035,7 +2962,7 @@
         <v>0.15483870999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29859520000000001</v>
       </c>
@@ -2061,7 +2988,7 @@
         <v>0.15180463</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29448505000000003</v>
       </c>
@@ -2087,7 +3014,7 @@
         <v>0.16106312</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.30150205000000002</v>
       </c>
@@ -2113,7 +3040,7 @@
         <v>0.15566682000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.30310192000000002</v>
       </c>
@@ -2139,7 +3066,7 @@
         <v>0.16051206000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.30333028000000001</v>
       </c>
@@ -2165,7 +3092,7 @@
         <v>0.16376413000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.31024195999999998</v>
       </c>
@@ -2191,7 +3118,7 @@
         <v>0.16121975</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.32696078000000001</v>
       </c>
@@ -2217,7 +3144,7 @@
         <v>0.16446078</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.31938984999999998</v>
       </c>
@@ -2243,7 +3170,7 @@
         <v>0.16168964999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.33510179000000001</v>
       </c>
@@ -2269,7 +3196,7 @@
         <v>0.16533004000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32786884999999999</v>
       </c>
@@ -2295,7 +3222,7 @@
         <v>0.15914249999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.32609421999999999</v>
       </c>
@@ -2327,6 +3254,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42333228-403B-7F4C-BA26-71F42800C60A}">
+  <dimension ref="A3:A43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1575</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5418AFA3-7BE2-40D6-B428-AEBC912691F4}">
   <dimension ref="A1:J39"/>
   <sheetViews>
@@ -2334,14 +3466,14 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2349,7 +3481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2375,7 +3507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.33362050999999998</v>
       </c>
@@ -2401,7 +3533,7 @@
         <v>0.13948717999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.31823384999999998</v>
       </c>
@@ -2427,7 +3559,7 @@
         <v>0.13736713</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.32943302000000002</v>
       </c>
@@ -2453,7 +3585,7 @@
         <v>0.13553196000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.32304676999999998</v>
       </c>
@@ -2479,7 +3611,7 @@
         <v>0.14158498999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.30914533</v>
       </c>
@@ -2505,7 +3637,7 @@
         <v>0.12371134</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.28972652999999998</v>
       </c>
@@ -2531,7 +3663,7 @@
         <v>0.11914265</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.30600398000000001</v>
       </c>
@@ -2557,7 +3689,7 @@
         <v>0.12803181</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.27075038000000001</v>
       </c>
@@ -2583,7 +3715,7 @@
         <v>0.13584362</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26014481</v>
       </c>
@@ -2609,7 +3741,7 @@
         <v>0.13290426</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.25827051000000001</v>
       </c>
@@ -2635,7 +3767,7 @@
         <v>0.13250554</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.25882857999999997</v>
       </c>
@@ -2661,7 +3793,7 @@
         <v>0.13473504</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26004906999999999</v>
       </c>
@@ -2687,7 +3819,7 @@
         <v>0.13566070999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26376770999999999</v>
       </c>
@@ -2713,7 +3845,7 @@
         <v>0.14060877999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26906546999999997</v>
       </c>
@@ -2739,7 +3871,7 @@
         <v>0.14204326</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27410029000000002</v>
       </c>
@@ -2765,7 +3897,7 @@
         <v>0.14430678</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.2836822</v>
       </c>
@@ -2791,7 +3923,7 @@
         <v>0.15033850000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28821972000000001</v>
       </c>
@@ -2817,7 +3949,7 @@
         <v>0.15201853000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.29324736000000001</v>
       </c>
@@ -2843,7 +3975,7 @@
         <v>0.15376840999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.28451009999999999</v>
       </c>
@@ -2869,7 +4001,7 @@
         <v>0.15555073</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.28960216</v>
       </c>
@@ -2895,7 +4027,7 @@
         <v>0.15547938</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29367304</v>
       </c>
@@ -2921,7 +4053,7 @@
         <v>0.15694268</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.28868527999999999</v>
       </c>
@@ -2947,7 +4079,7 @@
         <v>0.15495418999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29712245999999998</v>
       </c>
@@ -2973,7 +4105,7 @@
         <v>0.15784073000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.29478314</v>
       </c>
@@ -2999,7 +4131,7 @@
         <v>0.16244349</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.30189136</v>
       </c>
@@ -3025,7 +4157,7 @@
         <v>0.16002421</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.30255769999999998</v>
       </c>
@@ -3051,7 +4183,7 @@
         <v>0.16044916000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.31600928</v>
       </c>
@@ -3077,7 +4209,7 @@
         <v>0.16600928000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.31857101999999998</v>
       </c>
@@ -3103,7 +4235,7 @@
         <v>0.16626028000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.32132192999999998</v>
       </c>
@@ -3129,7 +4261,7 @@
         <v>0.15805189</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32438053999999999</v>
       </c>
@@ -3155,7 +4287,7 @@
         <v>0.16445396000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.31789474000000001</v>
       </c>
@@ -3186,7 +4318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FF4068-F092-4FA3-899F-F95F2AA20693}">
   <dimension ref="A1:J39"/>
   <sheetViews>
@@ -3194,14 +4326,14 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3209,7 +4341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3235,7 +4367,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.34167161000000001</v>
       </c>
@@ -3261,7 +4393,7 @@
         <v>0.13965619000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.31370810999999998</v>
       </c>
@@ -3287,7 +4419,7 @@
         <v>0.13802270999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.33762994000000002</v>
       </c>
@@ -3313,7 +4445,7 @@
         <v>0.13780814</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.31879078999999999</v>
       </c>
@@ -3339,7 +4471,7 @@
         <v>0.14455514</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.30993711000000002</v>
       </c>
@@ -3365,7 +4497,7 @@
         <v>0.13450734</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.28888889000000001</v>
       </c>
@@ -3391,7 +4523,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.28399720000000001</v>
       </c>
@@ -3417,7 +4549,7 @@
         <v>0.11069182</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.27711075000000002</v>
       </c>
@@ -3443,7 +4575,7 @@
         <v>0.13269127999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26501271999999998</v>
       </c>
@@ -3469,7 +4601,7 @@
         <v>0.13282442999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.26241593000000002</v>
       </c>
@@ -3495,7 +4627,7 @@
         <v>0.13155770999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26059362000000003</v>
       </c>
@@ -3521,7 +4653,7 @@
         <v>0.1343538</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26204830000000001</v>
       </c>
@@ -3547,7 +4679,7 @@
         <v>0.13322945999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26498466999999998</v>
       </c>
@@ -3573,7 +4705,7 @@
         <v>0.14015562000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26956318000000001</v>
       </c>
@@ -3599,7 +4731,7 @@
         <v>0.14170972000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27463185000000001</v>
       </c>
@@ -3625,7 +4757,7 @@
         <v>0.14509031999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.28448783</v>
       </c>
@@ -3651,7 +4783,7 @@
         <v>0.14747513000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28883845000000002</v>
       </c>
@@ -3677,7 +4809,7 @@
         <v>0.14984111</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.29209417999999998</v>
       </c>
@@ -3703,7 +4835,7 @@
         <v>0.15018988</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.29092067999999999</v>
       </c>
@@ -3729,7 +4861,7 @@
         <v>0.15074865000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.29646939</v>
       </c>
@@ -3755,7 +4887,7 @@
         <v>0.15971552</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29336092000000002</v>
       </c>
@@ -3781,7 +4913,7 @@
         <v>0.15450939999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29697481999999997</v>
       </c>
@@ -3807,7 +4939,7 @@
         <v>0.15940509999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29654285000000002</v>
       </c>
@@ -3833,7 +4965,7 @@
         <v>0.16038432</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.30336994</v>
       </c>
@@ -3859,7 +4991,7 @@
         <v>0.15956076999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.30869029999999997</v>
       </c>
@@ -3885,7 +5017,7 @@
         <v>0.16427692999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.31396192000000001</v>
       </c>
@@ -3911,7 +5043,7 @@
         <v>0.16518585999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.32179967999999998</v>
       </c>
@@ -3937,7 +5069,7 @@
         <v>0.16445635</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.32116973999999998</v>
       </c>
@@ -3963,7 +5095,7 @@
         <v>0.16181393999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.32430783000000002</v>
       </c>
@@ -3989,7 +5121,7 @@
         <v>0.16054066</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32759178</v>
       </c>
@@ -4015,7 +5147,7 @@
         <v>0.16374970999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32193158999999999</v>
       </c>
@@ -4046,7 +5178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CD98FB-A331-48CA-AB8A-6C15D9AAF3D0}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -4054,14 +5186,14 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4069,7 +5201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4095,7 +5227,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.34416404</v>
       </c>
@@ -4121,7 +5253,7 @@
         <v>0.12933754</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.30636992000000002</v>
       </c>
@@ -4147,7 +5279,7 @@
         <v>0.14090559999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.34730538999999999</v>
       </c>
@@ -4173,7 +5305,7 @@
         <v>0.12865697000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.33931623999999999</v>
       </c>
@@ -4199,7 +5331,7 @@
         <v>0.15341879999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.32685015000000001</v>
       </c>
@@ -4225,7 +5357,7 @@
         <v>0.13211009000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.30519308000000001</v>
       </c>
@@ -4251,7 +5383,7 @@
         <v>0.13848202000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.29375469999999998</v>
       </c>
@@ -4277,7 +5409,7 @@
         <v>0.13032355000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26918048</v>
       </c>
@@ -4303,7 +5435,7 @@
         <v>0.13367797000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.26853373000000003</v>
       </c>
@@ -4329,7 +5461,7 @@
         <v>0.13388986</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26214633999999998</v>
       </c>
@@ -4355,7 +5487,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26192703000000001</v>
       </c>
@@ -4381,7 +5513,7 @@
         <v>0.13395697000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26326393999999997</v>
       </c>
@@ -4407,7 +5539,7 @@
         <v>0.13610924999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26335894999999998</v>
       </c>
@@ -4433,7 +5565,7 @@
         <v>0.13901206999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27062341000000001</v>
       </c>
@@ -4459,7 +5591,7 @@
         <v>0.14164544000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.27808702000000002</v>
       </c>
@@ -4485,7 +5617,7 @@
         <v>0.14386004999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28527353</v>
       </c>
@@ -4511,7 +5643,7 @@
         <v>0.14800047</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.29173006000000001</v>
       </c>
@@ -4537,7 +5669,7 @@
         <v>0.15234355999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.29256432999999998</v>
       </c>
@@ -4563,7 +5695,7 @@
         <v>0.15186862000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.29073042999999998</v>
       </c>
@@ -4589,7 +5721,7 @@
         <v>0.15342285999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29402662000000002</v>
       </c>
@@ -4615,7 +5747,7 @@
         <v>0.15685546</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29493201000000002</v>
       </c>
@@ -4641,7 +5773,7 @@
         <v>0.15710753999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29540613999999998</v>
       </c>
@@ -4667,7 +5799,7 @@
         <v>0.15793990999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.30221932000000001</v>
       </c>
@@ -4693,7 +5825,7 @@
         <v>0.16031332000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.29548410000000003</v>
       </c>
@@ -4719,7 +5851,7 @@
         <v>0.15828501</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.30537913</v>
       </c>
@@ -4745,7 +5877,7 @@
         <v>0.15761504000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.32058420999999998</v>
       </c>
@@ -4771,7 +5903,7 @@
         <v>0.16522136000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.31473277999999999</v>
       </c>
@@ -4797,7 +5929,7 @@
         <v>0.16240602000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.31437598999999999</v>
       </c>
@@ -4823,7 +5955,7 @@
         <v>0.16382305999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32120472</v>
       </c>
@@ -4849,7 +5981,7 @@
         <v>0.16507937</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32572783999999999</v>
       </c>
@@ -4875,7 +6007,7 @@
         <v>0.15803321000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.32102965</v>
       </c>
@@ -4906,7 +6038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA542B6F-8910-4C27-A3B9-56233D36282B}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -4914,14 +6046,14 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4929,7 +6061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4955,7 +6087,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.36071428999999999</v>
       </c>
@@ -4981,7 +6113,7 @@
         <v>0.13392857</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.31332654999999998</v>
       </c>
@@ -5007,7 +6139,7 @@
         <v>0.13997965000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.33333332999999998</v>
       </c>
@@ -5033,7 +6165,7 @@
         <v>0.14457830999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.31369295000000003</v>
       </c>
@@ -5059,7 +6191,7 @@
         <v>0.12448133</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.35149786</v>
       </c>
@@ -5085,7 +6217,7 @@
         <v>0.15406561999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.30482114999999999</v>
       </c>
@@ -5111,7 +6243,7 @@
         <v>0.14681182000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.32920354000000002</v>
       </c>
@@ -5137,7 +6269,7 @@
         <v>0.10088496</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.27376594999999998</v>
       </c>
@@ -5163,7 +6295,7 @@
         <v>0.13355518999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.26932171999999999</v>
       </c>
@@ -5189,7 +6321,7 @@
         <v>0.13275254</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26560477999999998</v>
       </c>
@@ -5215,7 +6347,7 @@
         <v>0.1315414</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.25926145</v>
       </c>
@@ -5241,7 +6373,7 @@
         <v>0.1371935</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26297029999999999</v>
       </c>
@@ -5267,7 +6399,7 @@
         <v>0.13691655</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.27035616000000001</v>
       </c>
@@ -5293,7 +6425,7 @@
         <v>0.14268492999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.266984</v>
       </c>
@@ -5319,7 +6451,7 @@
         <v>0.14248314000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.27504271000000002</v>
       </c>
@@ -5345,7 +6477,7 @@
         <v>0.14561703000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.27714935000000002</v>
       </c>
@@ -5371,7 +6503,7 @@
         <v>0.14386950000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.29157327</v>
       </c>
@@ -5397,7 +6529,7 @@
         <v>0.15552788000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.29173756000000001</v>
       </c>
@@ -5423,7 +6555,7 @@
         <v>0.15065608999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.29383202000000003</v>
       </c>
@@ -5449,7 +6581,7 @@
         <v>0.15367454</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.28858843000000001</v>
       </c>
@@ -5475,7 +6607,7 @@
         <v>0.16700919</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29901823</v>
       </c>
@@ -5501,7 +6633,7 @@
         <v>0.16227209000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29620837</v>
       </c>
@@ -5527,7 +6659,7 @@
         <v>0.16102868000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.30382848000000001</v>
       </c>
@@ -5553,7 +6685,7 @@
         <v>0.15763144000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.30746543999999998</v>
       </c>
@@ -5579,7 +6711,7 @@
         <v>0.16058986</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.31291764</v>
       </c>
@@ -5605,7 +6737,7 @@
         <v>0.16173654000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.31487532000000001</v>
       </c>
@@ -5631,7 +6763,7 @@
         <v>0.16268272</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.31967870999999998</v>
       </c>
@@ -5657,7 +6789,7 @@
         <v>0.16064257000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.32507385999999999</v>
       </c>
@@ -5683,7 +6815,7 @@
         <v>0.16545203999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.33176661000000002</v>
       </c>
@@ -5709,7 +6841,7 @@
         <v>0.16677471999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32194102000000002</v>
       </c>
@@ -5735,7 +6867,7 @@
         <v>0.15946455000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.31843920999999997</v>
       </c>
@@ -5766,7 +6898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33ECEDF-2720-4E23-99EF-4313233ABC9E}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -5774,14 +6906,14 @@
       <selection activeCell="G5" sqref="G5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5789,7 +6921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5815,7 +6947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.37279305000000001</v>
       </c>
@@ -5841,7 +6973,7 @@
         <v>0.14587554</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.32328767000000003</v>
       </c>
@@ -5867,7 +6999,7 @@
         <v>0.15671233000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.32489083000000002</v>
       </c>
@@ -5893,7 +7025,7 @@
         <v>0.10247452999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.35333333</v>
       </c>
@@ -5919,7 +7051,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.31386860999999999</v>
       </c>
@@ -5945,7 +7077,7 @@
         <v>0.11824817999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.36715788999999999</v>
       </c>
@@ -5971,7 +7103,7 @@
         <v>0.13305263000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.31295337000000001</v>
       </c>
@@ -5997,7 +7129,7 @@
         <v>0.11606218</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26335591000000003</v>
       </c>
@@ -6023,7 +7155,7 @@
         <v>0.13423626999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.26447412999999997</v>
       </c>
@@ -6049,7 +7181,7 @@
         <v>0.13840356000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26225962000000003</v>
       </c>
@@ -6075,7 +7207,7 @@
         <v>0.12932692000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.26105971</v>
       </c>
@@ -6101,7 +7233,7 @@
         <v>0.13097840999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26900584999999999</v>
       </c>
@@ -6127,7 +7259,7 @@
         <v>0.13588517</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.27325611</v>
       </c>
@@ -6153,7 +7285,7 @@
         <v>0.14517374999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.27372549000000002</v>
       </c>
@@ -6179,7 +7311,7 @@
         <v>0.14411765000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.28583078000000001</v>
       </c>
@@ -6205,7 +7337,7 @@
         <v>0.14169214999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.29090908999999998</v>
       </c>
@@ -6231,7 +7363,7 @@
         <v>0.14707973999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.28541989000000001</v>
       </c>
@@ -6257,7 +7389,7 @@
         <v>0.15126223999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.28242778000000002</v>
       </c>
@@ -6283,7 +7415,7 @@
         <v>0.15457196000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.28325106999999999</v>
       </c>
@@ -6309,7 +7441,7 @@
         <v>0.15136558</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29312789</v>
       </c>
@@ -6335,7 +7467,7 @@
         <v>0.14791988</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.30067459000000002</v>
       </c>
@@ -6361,7 +7493,7 @@
         <v>0.15367812</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29095385000000001</v>
       </c>
@@ -6387,7 +7519,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.29612842</v>
       </c>
@@ -6413,7 +7545,7 @@
         <v>0.16191375999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.29742896000000002</v>
       </c>
@@ -6439,7 +7571,7 @@
         <v>0.15588632999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.29266693999999999</v>
       </c>
@@ -6465,7 +7597,7 @@
         <v>0.16091765999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.3293913</v>
       </c>
@@ -6491,7 +7623,7 @@
         <v>0.16173913000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.31761475</v>
       </c>
@@ -6517,7 +7649,7 @@
         <v>0.16759514</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.31137371000000003</v>
       </c>
@@ -6543,7 +7675,7 @@
         <v>0.16809452999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32154440000000001</v>
       </c>
@@ -6569,7 +7701,7 @@
         <v>0.16247104000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32822891999999998</v>
       </c>
@@ -6595,7 +7727,7 @@
         <v>0.15839133999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.31357924999999998</v>
       </c>
@@ -6626,7 +7758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F56B74-9E62-4622-9A68-4FC8248BB2CE}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -6634,9 +7766,9 @@
       <selection activeCell="G5" sqref="G5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6647,7 +7779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6655,7 +7787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6681,7 +7813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8.1811540000000002E-2</v>
       </c>
@@ -6707,7 +7839,7 @@
         <v>6.6617969999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.23035994000000001</v>
       </c>
@@ -6733,7 +7865,7 @@
         <v>0.15899843999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.25974026</v>
       </c>
@@ -6759,7 +7891,7 @@
         <v>0.17454544999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.19114503999999999</v>
       </c>
@@ -6785,7 +7917,7 @@
         <v>7.8167940000000005E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.19207179999999999</v>
       </c>
@@ -6811,7 +7943,7 @@
         <v>3.111444E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.23625731</v>
       </c>
@@ -6837,7 +7969,7 @@
         <v>3.274854E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.24018692</v>
       </c>
@@ -6863,7 +7995,7 @@
         <v>3.3644859999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.27180676999999998</v>
       </c>
@@ -6889,7 +8021,7 @@
         <v>0.13641526000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.27027649999999998</v>
       </c>
@@ -6915,7 +8047,7 @@
         <v>0.13271889000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.26112596999999999</v>
       </c>
@@ -6941,7 +8073,7 @@
         <v>0.13202027</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.25972498999999999</v>
       </c>
@@ -6967,7 +8099,7 @@
         <v>0.13326336</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26019457000000001</v>
       </c>
@@ -6993,7 +8125,7 @@
         <v>0.13421158999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26314733000000001</v>
       </c>
@@ -7019,7 +8151,7 @@
         <v>0.13801685999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.26787916000000001</v>
       </c>
@@ -7045,7 +8177,7 @@
         <v>0.14113368000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.27324810999999999</v>
       </c>
@@ -7071,7 +8203,7 @@
         <v>0.14401252</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28006766</v>
       </c>
@@ -7097,7 +8229,7 @@
         <v>0.14649424</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.28368243999999998</v>
       </c>
@@ -7123,7 +8255,7 @@
         <v>0.14903258999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.2896628</v>
       </c>
@@ -7149,7 +8281,7 @@
         <v>0.15168601000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.28864457999999998</v>
       </c>
@@ -7175,7 +8307,7 @@
         <v>0.15359955</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.31815696999999998</v>
       </c>
@@ -7201,7 +8333,7 @@
         <v>0.16493557</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29906184000000002</v>
       </c>
@@ -7227,7 +8359,7 @@
         <v>0.15638521999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29753355999999997</v>
       </c>
@@ -7253,7 +8385,7 @@
         <v>0.15953792999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.30042003</v>
       </c>
@@ -7279,7 +8411,7 @@
         <v>0.15896606999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.30200285999999998</v>
       </c>
@@ -7305,7 +8437,7 @@
         <v>0.16552217</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.30469435</v>
       </c>
@@ -7331,7 +8463,7 @@
         <v>0.16348842</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.31589877</v>
       </c>
@@ -7357,7 +8489,7 @@
         <v>0.16569327</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.32039131999999998</v>
       </c>
@@ -7383,7 +8515,7 @@
         <v>0.16541322999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.32402802000000003</v>
       </c>
@@ -7409,7 +8541,7 @@
         <v>0.16339458000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32357844000000002</v>
       </c>
@@ -7435,7 +8567,7 @@
         <v>0.16491190999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32425189999999998</v>
       </c>
@@ -7461,7 +8593,7 @@
         <v>0.16328718</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.31866496</v>
       </c>
@@ -7492,7 +8624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2694D348-F552-4FCA-971C-0A5A9ADA03D8}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -7500,9 +8632,9 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -7513,7 +8645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -7521,7 +8653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -7547,7 +8679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.32536313</v>
       </c>
@@ -7573,7 +8705,7 @@
         <v>0.12670391</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.32</v>
       </c>
@@ -7599,7 +8731,7 @@
         <v>0.14295082000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.33414254999999998</v>
       </c>
@@ -7625,7 +8757,7 @@
         <v>0.13071895</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.32148731000000003</v>
       </c>
@@ -7651,7 +8783,7 @@
         <v>0.13671791</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.28786177000000002</v>
       </c>
@@ -7677,7 +8809,7 @@
         <v>0.13062635</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.31228615999999998</v>
       </c>
@@ -7703,7 +8835,7 @@
         <v>0.13851737</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.30970816000000001</v>
       </c>
@@ -7729,7 +8861,7 @@
         <v>0.12078618000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.26941416000000001</v>
       </c>
@@ -7755,7 +8887,7 @@
         <v>0.13609679999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.26427701999999997</v>
       </c>
@@ -7781,7 +8913,7 @@
         <v>0.13859940000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.25780839</v>
       </c>
@@ -7807,7 +8939,7 @@
         <v>0.13481872</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.25999612</v>
       </c>
@@ -7833,7 +8965,7 @@
         <v>0.13674617</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.26280896999999998</v>
       </c>
@@ -7859,7 +8991,7 @@
         <v>0.13381873999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.26251424000000001</v>
       </c>
@@ -7885,7 +9017,7 @@
         <v>0.13786555</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.26935284999999998</v>
       </c>
@@ -7911,7 +9043,7 @@
         <v>0.14421743000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.27371149</v>
       </c>
@@ -7937,7 +9069,7 @@
         <v>0.1469046</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.28374426000000003</v>
       </c>
@@ -7963,7 +9095,7 @@
         <v>0.15036823999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.28625696</v>
       </c>
@@ -7989,7 +9121,7 @@
         <v>0.15063857999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.28963435999999998</v>
       </c>
@@ -8015,7 +9147,7 @@
         <v>0.15340685000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.28378829999999999</v>
       </c>
@@ -8041,7 +9173,7 @@
         <v>0.15777158999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.29376601000000002</v>
       </c>
@@ -8067,7 +9199,7 @@
         <v>0.15508113000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.29608540999999999</v>
       </c>
@@ -8093,7 +9225,7 @@
         <v>0.15703914999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.29966200999999998</v>
       </c>
@@ -8119,7 +9251,7 @@
         <v>0.15870682999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.29755951000000003</v>
       </c>
@@ -8145,7 +9277,7 @@
         <v>0.16161494000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.31028917</v>
       </c>
@@ -8171,7 +9303,7 @@
         <v>0.16207128000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.31152036</v>
       </c>
@@ -8197,7 +9329,7 @@
         <v>0.16599141000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.31354417000000001</v>
       </c>
@@ -8223,7 +9355,7 @@
         <v>0.16610686999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.3225498</v>
       </c>
@@ -8249,7 +9381,7 @@
         <v>0.16175299000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.31862464000000001</v>
       </c>
@@ -8275,7 +9407,7 @@
         <v>0.16382044000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.32795436</v>
       </c>
@@ -8301,7 +9433,7 @@
         <v>0.17000815</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.32333332999999997</v>
       </c>
@@ -8327,7 +9459,7 @@
         <v>0.16750000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.32615938999999999</v>
       </c>
@@ -8351,872 +9483,6 @@
       </c>
       <c r="J40">
         <v>0.1710941</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2FAC0B-EE3B-42E4-A7E5-2FA82B54F342}">
-  <dimension ref="A1:J40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0.33089004999999999</v>
-      </c>
-      <c r="B6">
-        <v>0.20646750999999999</v>
-      </c>
-      <c r="C6">
-        <v>0.28629504</v>
-      </c>
-      <c r="D6">
-        <v>0.28629504</v>
-      </c>
-      <c r="G6">
-        <v>0.12811826000000001</v>
-      </c>
-      <c r="H6">
-        <v>0.14733599999999999</v>
-      </c>
-      <c r="I6">
-        <v>0.14758238000000001</v>
-      </c>
-      <c r="J6">
-        <v>0.13575608</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.32077763999999998</v>
-      </c>
-      <c r="B7">
-        <v>0.21652490999999999</v>
-      </c>
-      <c r="C7">
-        <v>0.28092345000000002</v>
-      </c>
-      <c r="D7">
-        <v>0.29161604000000002</v>
-      </c>
-      <c r="G7">
-        <v>0.13584446999999999</v>
-      </c>
-      <c r="H7">
-        <v>0.14167679</v>
-      </c>
-      <c r="I7">
-        <v>0.14872418000000001</v>
-      </c>
-      <c r="J7">
-        <v>0.13803159000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0.31667183999999998</v>
-      </c>
-      <c r="B8">
-        <v>0.2116113</v>
-      </c>
-      <c r="C8">
-        <v>0.29655387</v>
-      </c>
-      <c r="D8">
-        <v>0.28810928000000002</v>
-      </c>
-      <c r="G8">
-        <v>0.13660354</v>
-      </c>
-      <c r="H8">
-        <v>0.13635517</v>
-      </c>
-      <c r="I8">
-        <v>0.13983234999999999</v>
-      </c>
-      <c r="J8">
-        <v>0.13585843</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0.32184238999999998</v>
-      </c>
-      <c r="B9">
-        <v>0.21907161</v>
-      </c>
-      <c r="C9">
-        <v>0.28096438000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.28038863000000003</v>
-      </c>
-      <c r="G9">
-        <v>0.13098236999999999</v>
-      </c>
-      <c r="H9">
-        <v>0.14134580999999999</v>
-      </c>
-      <c r="I9">
-        <v>0.14019430999999999</v>
-      </c>
-      <c r="J9">
-        <v>0.12810363</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.30941286000000001</v>
-      </c>
-      <c r="B10">
-        <v>0.20577819</v>
-      </c>
-      <c r="C10">
-        <v>0.27250699</v>
-      </c>
-      <c r="D10">
-        <v>0.27287978000000002</v>
-      </c>
-      <c r="G10">
-        <v>0.13159366</v>
-      </c>
-      <c r="H10">
-        <v>0.14464119</v>
-      </c>
-      <c r="I10">
-        <v>0.13643989000000001</v>
-      </c>
-      <c r="J10">
-        <v>0.14575954999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0.28771482999999998</v>
-      </c>
-      <c r="B11">
-        <v>0.19554424000000001</v>
-      </c>
-      <c r="C11">
-        <v>0.23169955</v>
-      </c>
-      <c r="D11">
-        <v>0.24595798999999999</v>
-      </c>
-      <c r="G11">
-        <v>9.9299810000000002E-2</v>
-      </c>
-      <c r="H11">
-        <v>0.13952896000000001</v>
-      </c>
-      <c r="I11">
-        <v>0.11763208</v>
-      </c>
-      <c r="J11">
-        <v>0.12068746</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0.29838998</v>
-      </c>
-      <c r="B12">
-        <v>0.18175313000000001</v>
-      </c>
-      <c r="C12">
-        <v>0.26833631000000002</v>
-      </c>
-      <c r="D12">
-        <v>0.24758496999999999</v>
-      </c>
-      <c r="G12">
-        <v>0.11234347</v>
-      </c>
-      <c r="H12">
-        <v>0.12593918000000001</v>
-      </c>
-      <c r="I12">
-        <v>0.14311270000000001</v>
-      </c>
-      <c r="J12">
-        <v>0.12307692000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0.26548012999999998</v>
-      </c>
-      <c r="B15">
-        <v>0.22094370999999999</v>
-      </c>
-      <c r="C15">
-        <v>0.23038079</v>
-      </c>
-      <c r="D15">
-        <v>0.23791391000000001</v>
-      </c>
-      <c r="G15">
-        <v>0.12847681999999999</v>
-      </c>
-      <c r="H15">
-        <v>0.13899006999999999</v>
-      </c>
-      <c r="I15">
-        <v>0.12152317999999999</v>
-      </c>
-      <c r="J15">
-        <v>0.13269868000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>0.27439933999999999</v>
-      </c>
-      <c r="B16">
-        <v>0.22336370999999999</v>
-      </c>
-      <c r="C16">
-        <v>0.23491537000000001</v>
-      </c>
-      <c r="D16">
-        <v>0.24627767</v>
-      </c>
-      <c r="G16">
-        <v>0.12934075</v>
-      </c>
-      <c r="H16">
-        <v>0.13871464</v>
-      </c>
-      <c r="I16">
-        <v>0.11987217</v>
-      </c>
-      <c r="J16">
-        <v>0.13454847</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>0.26748034999999998</v>
-      </c>
-      <c r="B17">
-        <v>0.22184003999999999</v>
-      </c>
-      <c r="C17">
-        <v>0.22901526</v>
-      </c>
-      <c r="D17">
-        <v>0.24114656000000001</v>
-      </c>
-      <c r="G17">
-        <v>0.12737863999999999</v>
-      </c>
-      <c r="H17">
-        <v>0.13618122999999999</v>
-      </c>
-      <c r="I17">
-        <v>0.11968562000000001</v>
-      </c>
-      <c r="J17">
-        <v>0.13129911999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>0.26209485999999999</v>
-      </c>
-      <c r="B18">
-        <v>0.21396032000000001</v>
-      </c>
-      <c r="C18">
-        <v>0.22650012</v>
-      </c>
-      <c r="D18">
-        <v>0.23459874</v>
-      </c>
-      <c r="G18">
-        <v>0.12722670999999999</v>
-      </c>
-      <c r="H18">
-        <v>0.13480284000000001</v>
-      </c>
-      <c r="I18">
-        <v>0.12245898</v>
-      </c>
-      <c r="J18">
-        <v>0.13251694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>0.26120821999999999</v>
-      </c>
-      <c r="B19">
-        <v>0.21416742999999999</v>
-      </c>
-      <c r="C19">
-        <v>0.22913217</v>
-      </c>
-      <c r="D19">
-        <v>0.23643053999999999</v>
-      </c>
-      <c r="G19">
-        <v>0.13014413</v>
-      </c>
-      <c r="H19">
-        <v>0.13750382999999999</v>
-      </c>
-      <c r="I19">
-        <v>0.12486967</v>
-      </c>
-      <c r="J19">
-        <v>0.13351732999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>0.26752530000000002</v>
-      </c>
-      <c r="B20">
-        <v>0.22079117000000001</v>
-      </c>
-      <c r="C20">
-        <v>0.23563323999999999</v>
-      </c>
-      <c r="D20">
-        <v>0.24225698000000001</v>
-      </c>
-      <c r="G20">
-        <v>0.13529591999999999</v>
-      </c>
-      <c r="H20">
-        <v>0.14308493999999999</v>
-      </c>
-      <c r="I20">
-        <v>0.12977614000000001</v>
-      </c>
-      <c r="J20">
-        <v>0.13854646000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>0.27011866000000001</v>
-      </c>
-      <c r="B21">
-        <v>0.22357836</v>
-      </c>
-      <c r="C21">
-        <v>0.24083834000000001</v>
-      </c>
-      <c r="D21">
-        <v>0.24650948</v>
-      </c>
-      <c r="G21">
-        <v>0.13826475999999999</v>
-      </c>
-      <c r="H21">
-        <v>0.14652488999999999</v>
-      </c>
-      <c r="I21">
-        <v>0.13321005</v>
-      </c>
-      <c r="J21">
-        <v>0.14140854</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>0.27199624999999999</v>
-      </c>
-      <c r="B22">
-        <v>0.22459208</v>
-      </c>
-      <c r="C22">
-        <v>0.2427668</v>
-      </c>
-      <c r="D22">
-        <v>0.25319697000000002</v>
-      </c>
-      <c r="G22">
-        <v>0.13859004999999999</v>
-      </c>
-      <c r="H22">
-        <v>0.14758373</v>
-      </c>
-      <c r="I22">
-        <v>0.13434304</v>
-      </c>
-      <c r="J22">
-        <v>0.14383636999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>0.28171053000000001</v>
-      </c>
-      <c r="B23">
-        <v>0.23190789000000001</v>
-      </c>
-      <c r="C23">
-        <v>0.24881579000000001</v>
-      </c>
-      <c r="D23">
-        <v>0.26078947000000002</v>
-      </c>
-      <c r="G23">
-        <v>0.14467105</v>
-      </c>
-      <c r="H23">
-        <v>0.15269737</v>
-      </c>
-      <c r="I23">
-        <v>0.13717104999999999</v>
-      </c>
-      <c r="J23">
-        <v>0.14611842</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>0.28868268000000002</v>
-      </c>
-      <c r="B24">
-        <v>0.23567774</v>
-      </c>
-      <c r="C24">
-        <v>0.25600555000000003</v>
-      </c>
-      <c r="D24">
-        <v>0.26627351999999999</v>
-      </c>
-      <c r="G24">
-        <v>0.14513919</v>
-      </c>
-      <c r="H24">
-        <v>0.15367270999999999</v>
-      </c>
-      <c r="I24">
-        <v>0.13924204000000001</v>
-      </c>
-      <c r="J24">
-        <v>0.14964876999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>0.29242199000000002</v>
-      </c>
-      <c r="B25">
-        <v>0.24279345999999999</v>
-      </c>
-      <c r="C25">
-        <v>0.25995541999999999</v>
-      </c>
-      <c r="D25">
-        <v>0.27280831999999999</v>
-      </c>
-      <c r="G25">
-        <v>0.14977712000000001</v>
-      </c>
-      <c r="H25">
-        <v>0.15713224000000001</v>
-      </c>
-      <c r="I25">
-        <v>0.14108470000000001</v>
-      </c>
-      <c r="J25">
-        <v>0.15022288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>0.29024002999999998</v>
-      </c>
-      <c r="B26">
-        <v>0.24278311999999999</v>
-      </c>
-      <c r="C26">
-        <v>0.26190123999999998</v>
-      </c>
-      <c r="D26">
-        <v>0.27433647</v>
-      </c>
-      <c r="G26">
-        <v>0.15099926</v>
-      </c>
-      <c r="H26">
-        <v>0.16064291</v>
-      </c>
-      <c r="I26">
-        <v>0.14194776000000001</v>
-      </c>
-      <c r="J26">
-        <v>0.15404461999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>0.30381944</v>
-      </c>
-      <c r="B29">
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="C29">
-        <v>0.26163194000000001</v>
-      </c>
-      <c r="D29">
-        <v>0.27916667000000001</v>
-      </c>
-      <c r="G29">
-        <v>0.15121528000000001</v>
-      </c>
-      <c r="H29">
-        <v>0.16371527999999999</v>
-      </c>
-      <c r="I29">
-        <v>0.15885416999999999</v>
-      </c>
-      <c r="J29">
-        <v>0.15468750000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>0.29318894000000001</v>
-      </c>
-      <c r="B30">
-        <v>0.25830721000000001</v>
-      </c>
-      <c r="C30">
-        <v>0.26058705999999998</v>
-      </c>
-      <c r="D30">
-        <v>0.28201767</v>
-      </c>
-      <c r="G30">
-        <v>0.14636648999999999</v>
-      </c>
-      <c r="H30">
-        <v>0.15822172000000001</v>
-      </c>
-      <c r="I30">
-        <v>0.1461385</v>
-      </c>
-      <c r="J30">
-        <v>0.15252209</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>0.29888334999999999</v>
-      </c>
-      <c r="B31">
-        <v>0.25801853000000002</v>
-      </c>
-      <c r="C31">
-        <v>0.26666666999999999</v>
-      </c>
-      <c r="D31">
-        <v>0.28168210999999999</v>
-      </c>
-      <c r="G31">
-        <v>0.15633167000000001</v>
-      </c>
-      <c r="H31">
-        <v>0.16345925</v>
-      </c>
-      <c r="I31">
-        <v>0.15452601999999999</v>
-      </c>
-      <c r="J31">
-        <v>0.15481112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>0.30217259000000002</v>
-      </c>
-      <c r="B32">
-        <v>0.25760408000000001</v>
-      </c>
-      <c r="C32">
-        <v>0.27080956</v>
-      </c>
-      <c r="D32">
-        <v>0.28508314000000001</v>
-      </c>
-      <c r="G32">
-        <v>0.15933973000000001</v>
-      </c>
-      <c r="H32">
-        <v>0.16380628999999999</v>
-      </c>
-      <c r="I32">
-        <v>0.15516446</v>
-      </c>
-      <c r="J32">
-        <v>0.15730063999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>0.30705962999999997</v>
-      </c>
-      <c r="B33">
-        <v>0.26319397</v>
-      </c>
-      <c r="C33">
-        <v>0.27777930000000001</v>
-      </c>
-      <c r="D33">
-        <v>0.28655243000000002</v>
-      </c>
-      <c r="G33">
-        <v>0.15824537</v>
-      </c>
-      <c r="H33">
-        <v>0.16394791</v>
-      </c>
-      <c r="I33">
-        <v>0.15824537</v>
-      </c>
-      <c r="J33">
-        <v>0.15901302</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>0.30741971000000001</v>
-      </c>
-      <c r="B34">
-        <v>0.27033697000000001</v>
-      </c>
-      <c r="C34">
-        <v>0.28071508000000001</v>
-      </c>
-      <c r="D34">
-        <v>0.29463692000000002</v>
-      </c>
-      <c r="G34">
-        <v>0.1642778</v>
-      </c>
-      <c r="H34">
-        <v>0.16971997999999999</v>
-      </c>
-      <c r="I34">
-        <v>0.15870907000000001</v>
-      </c>
-      <c r="J34">
-        <v>0.16174656000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>0.31991944999999999</v>
-      </c>
-      <c r="B35">
-        <v>0.28286624999999999</v>
-      </c>
-      <c r="C35">
-        <v>0.29065278999999999</v>
-      </c>
-      <c r="D35">
-        <v>0.30219836</v>
-      </c>
-      <c r="G35">
-        <v>0.16271186000000001</v>
-      </c>
-      <c r="H35">
-        <v>0.17210940999999999</v>
-      </c>
-      <c r="I35">
-        <v>0.16123510999999999</v>
-      </c>
-      <c r="J35">
-        <v>0.16338311999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>0.31824637</v>
-      </c>
-      <c r="B36">
-        <v>0.27761655000000002</v>
-      </c>
-      <c r="C36">
-        <v>0.28342081000000002</v>
-      </c>
-      <c r="D36">
-        <v>0.30392096000000002</v>
-      </c>
-      <c r="G36">
-        <v>0.16251930000000001</v>
-      </c>
-      <c r="H36">
-        <v>0.16696511</v>
-      </c>
-      <c r="I36">
-        <v>0.15844395999999999</v>
-      </c>
-      <c r="J36">
-        <v>0.15906144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>0.32429448</v>
-      </c>
-      <c r="B37">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C37">
-        <v>0.29006135</v>
-      </c>
-      <c r="D37">
-        <v>0.30380368000000002</v>
-      </c>
-      <c r="G37">
-        <v>0.16036810000000001</v>
-      </c>
-      <c r="H37">
-        <v>0.17092025</v>
-      </c>
-      <c r="I37">
-        <v>0.15840491000000001</v>
-      </c>
-      <c r="J37">
-        <v>0.16343558</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>0.33208990999999999</v>
-      </c>
-      <c r="B38">
-        <v>0.28592380000000001</v>
-      </c>
-      <c r="C38">
-        <v>0.29689144000000001</v>
-      </c>
-      <c r="D38">
-        <v>0.30862425999999998</v>
-      </c>
-      <c r="G38">
-        <v>0.16617249000000001</v>
-      </c>
-      <c r="H38">
-        <v>0.1733142</v>
-      </c>
-      <c r="I38">
-        <v>0.16349433999999999</v>
-      </c>
-      <c r="J38">
-        <v>0.16362187</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>0.33449812000000001</v>
-      </c>
-      <c r="B39">
-        <v>0.29133265000000003</v>
-      </c>
-      <c r="C39">
-        <v>0.30325454000000002</v>
-      </c>
-      <c r="D39">
-        <v>0.31147652999999997</v>
-      </c>
-      <c r="G39">
-        <v>0.16553614</v>
-      </c>
-      <c r="H39">
-        <v>0.1744433</v>
-      </c>
-      <c r="I39">
-        <v>0.16073998</v>
-      </c>
-      <c r="J39">
-        <v>0.16635833999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>0.32315044999999998</v>
-      </c>
-      <c r="B40">
-        <v>0.28308162999999997</v>
-      </c>
-      <c r="C40">
-        <v>0.29302236999999998</v>
-      </c>
-      <c r="D40">
-        <v>0.31091569000000002</v>
-      </c>
-      <c r="G40">
-        <v>0.16486331000000001</v>
-      </c>
-      <c r="H40">
-        <v>0.17403937999999999</v>
-      </c>
-      <c r="I40">
-        <v>0.16409863999999999</v>
-      </c>
-      <c r="J40">
-        <v>0.15935768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>